<commit_message>
Cluster annotations and marker gene objects
</commit_message>
<xml_diff>
--- a/data/cluster_annotations/T-NK_ambientRNAremoval_21.03.24.xlsx
+++ b/data/cluster_annotations/T-NK_ambientRNAremoval_21.03.24.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maksimovicjovana/Work/Projects/MCRI/melanie.neeland/paed-inflammation-CITEseq/data/cluster_annotations/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://petermacvic-my.sharepoint.com/personal/jovana_maksimovic_petermac_org/Documents/Work/Projects/MCRI/melanie.neeland/paed-inflammation-CITEseq/data/cluster_annotations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B3F167-E8FB-A349-A49B-C784AE3A756F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{65B3F167-E8FB-A349-A49B-C784AE3A756F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25B990E6-5866-AC4B-9980-07AD2C506CC9}"/>
   <bookViews>
-    <workbookView xWindow="3160" yWindow="1420" windowWidth="23260" windowHeight="12580" xr2:uid="{118F4D04-DBDD-48A2-B93E-A0E9387D109B}"/>
+    <workbookView xWindow="32740" yWindow="5540" windowWidth="23260" windowHeight="12580" xr2:uid="{118F4D04-DBDD-48A2-B93E-A0E9387D109B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="54">
   <si>
     <t>Cluster</t>
   </si>
   <si>
-    <t>Annotation</t>
-  </si>
-  <si>
     <t>Relevant marker genes</t>
   </si>
   <si>
@@ -188,13 +185,19 @@
     <t>CD4 T-rm</t>
   </si>
   <si>
-    <t>Broad</t>
-  </si>
-  <si>
     <t>CD8 T cells</t>
   </si>
   <si>
     <t>innate lymphocyte</t>
+  </si>
+  <si>
+    <t>ann_level_2</t>
+  </si>
+  <si>
+    <t>ann_level_1</t>
+  </si>
+  <si>
+    <t>ann_level_3</t>
   </si>
 </sst>
 </file>
@@ -259,9 +262,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -299,7 +302,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -405,7 +408,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -547,7 +550,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -555,380 +558,443 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D4CBBD9-A1AF-4D94-A696-F66536CC6EAC}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="22.83203125" customWidth="1"/>
-    <col min="4" max="4" width="61.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" customWidth="1"/>
+    <col min="2" max="4" width="22.83203125" customWidth="1"/>
+    <col min="5" max="5" width="61.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="F11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="E12" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="F13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="D14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" t="s">
         <v>33</v>
       </c>
-      <c r="E14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="D15" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="E15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="F15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="D16" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="E16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+      <c r="F16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D17" t="s">
         <v>13</v>
       </c>
       <c r="E17" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="F17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="D18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18" t="s">
         <v>47</v>
       </c>
-      <c r="E18" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D19" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E19" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="F19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="D20" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+      <c r="F20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="E21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="F21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" t="s">
+        <v>43</v>
+      </c>
+      <c r="F22" t="s">
         <v>44</v>
-      </c>
-      <c r="E22" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>